<commit_message>
Created initial mean variance py and test ipynb
</commit_message>
<xml_diff>
--- a/docs/optimization_assumptions_2022.xlsx
+++ b/docs/optimization_assumptions_2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hanmaccapital-my.sharepoint.com/personal/bmcdonald_hanmaccapital_com/Documents/Documents/Asset Allocation/2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenMcDonald\AppData\Local\Programs\Python\Python310\asset-allocation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{ED4CD753-DC72-41D8-B05A-0F4259FF36F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCF7DEA4-1125-4A24-B1C6-E4CBB30DB039}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA512FD-489B-4B7A-B1CE-5857B4F6564D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="4335" windowWidth="24690" windowHeight="11265" xr2:uid="{946E2936-A83E-4594-85B5-5ACA456D13A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{946E2936-A83E-4594-85B5-5ACA456D13A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Return and Risk" sheetId="8" r:id="rId1"/>
@@ -161,10 +161,10 @@
     <t>pvt_equity</t>
   </si>
   <si>
-    <t>return</t>
-  </si>
-  <si>
-    <t>risk</t>
+    <t>exp_return</t>
+  </si>
+  <si>
+    <t>exp_risk</t>
   </si>
 </sst>
 </file>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B73B3E-1EFF-4777-B31D-BF758A86895D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E2DCE2-EEC6-495F-9102-6D1C3295B13E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DfdKEj4yo2GbJ0l00mQE2lgPQbdh3NME8Wad3XvnFaqWlGZjAbWilvUdVgU+79Z91JJ42guntO8904InCui6jQ==" saltValue="EDTrKzpbD2aoD19JzS504A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kQTD3qK8YmLFzTKDBxzGaJiwk5EajW7CGuC3L6m1KIRX8NpV2hXZyiV4E5rZhk68+9/QOLPyDCvS22SM7m2Kzw==" saltValue="JWjGYFUmQdCM0KbIi6zmvw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>